<commit_message>
Update latest products Excel export
</commit_message>
<xml_diff>
--- a/data/excel/products_latest.xlsx
+++ b/data/excel/products_latest.xlsx
@@ -14,17 +14,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="97">
   <si>
     <t>platform</t>
   </si>
   <si>
+    <t>title</t>
+  </si>
+  <si>
     <t>url</t>
   </si>
   <si>
-    <t>title</t>
-  </si>
-  <si>
     <t>price</t>
   </si>
   <si>
@@ -43,13 +43,91 @@
     <t>amazon</t>
   </si>
   <si>
+    <t>Not Found</t>
+  </si>
+  <si>
     <t>https://www.amazon.com/s?k=gaming</t>
   </si>
   <si>
-    <t>Not Found</t>
-  </si>
-  <si>
-    <t>2,080.99</t>
+    <t>$1,274.99</t>
+  </si>
+  <si>
+    <t>$967.04</t>
+  </si>
+  <si>
+    <t>$1,499.99</t>
+  </si>
+  <si>
+    <t>$39.00</t>
+  </si>
+  <si>
+    <t>$54.00</t>
+  </si>
+  <si>
+    <t>$219.99</t>
+  </si>
+  <si>
+    <t>$39.98</t>
+  </si>
+  <si>
+    <t>$1,599.99</t>
+  </si>
+  <si>
+    <t>$24.99</t>
+  </si>
+  <si>
+    <t>$10.00</t>
+  </si>
+  <si>
+    <t>$389.99</t>
+  </si>
+  <si>
+    <t>$219.00</t>
+  </si>
+  <si>
+    <t>$1,479.99</t>
+  </si>
+  <si>
+    <t>$2,349.99</t>
+  </si>
+  <si>
+    <t>$759.99</t>
+  </si>
+  <si>
+    <t>$186.79</t>
+  </si>
+  <si>
+    <t>$849.99</t>
+  </si>
+  <si>
+    <t>$449.99</t>
+  </si>
+  <si>
+    <t>$810.99</t>
+  </si>
+  <si>
+    <t>$14.99</t>
+  </si>
+  <si>
+    <t>$674.98</t>
+  </si>
+  <si>
+    <t>$159.99</t>
+  </si>
+  <si>
+    <t>$349.00</t>
+  </si>
+  <si>
+    <t>$59.99</t>
+  </si>
+  <si>
+    <t>$249.00</t>
+  </si>
+  <si>
+    <t>$109.99</t>
+  </si>
+  <si>
+    <t>$49.24</t>
   </si>
   <si>
     <t>0%</t>
@@ -58,10 +136,175 @@
     <t>4.3</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>2025-09-01T02:06:11.516412</t>
+    <t>4.6</t>
+  </si>
+  <si>
+    <t>5.0</t>
+  </si>
+  <si>
+    <t>4.4</t>
+  </si>
+  <si>
+    <t>4.8</t>
+  </si>
+  <si>
+    <t>4.7</t>
+  </si>
+  <si>
+    <t>4.0</t>
+  </si>
+  <si>
+    <t>4.5</t>
+  </si>
+  <si>
+    <t>4.1</t>
+  </si>
+  <si>
+    <t>4.2</t>
+  </si>
+  <si>
+    <t>81</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>5,668</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>1,329</t>
+  </si>
+  <si>
+    <t>369</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>302</t>
+  </si>
+  <si>
+    <t>28,229</t>
+  </si>
+  <si>
+    <t>949</t>
+  </si>
+  <si>
+    <t>22,939</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>1,977</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>3,753</t>
+  </si>
+  <si>
+    <t>648</t>
+  </si>
+  <si>
+    <t>USB</t>
+  </si>
+  <si>
+    <t>39,512</t>
+  </si>
+  <si>
+    <t>520</t>
+  </si>
+  <si>
+    <t>18,152</t>
+  </si>
+  <si>
+    <t>1,006</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>1,262</t>
+  </si>
+  <si>
+    <t>10,620</t>
+  </si>
+  <si>
+    <t>1,164</t>
+  </si>
+  <si>
+    <t>9,496</t>
+  </si>
+  <si>
+    <t>21,581</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>1,934</t>
+  </si>
+  <si>
+    <t>1,470</t>
+  </si>
+  <si>
+    <t>34,529</t>
+  </si>
+  <si>
+    <t>8,465</t>
+  </si>
+  <si>
+    <t>457</t>
+  </si>
+  <si>
+    <t>747</t>
+  </si>
+  <si>
+    <t>101,275</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>8,405</t>
+  </si>
+  <si>
+    <t>748</t>
+  </si>
+  <si>
+    <t>14,314</t>
+  </si>
+  <si>
+    <t>4,963</t>
+  </si>
+  <si>
+    <t>2,301</t>
+  </si>
+  <si>
+    <t>24,092</t>
+  </si>
+  <si>
+    <t>31,392</t>
+  </si>
+  <si>
+    <t>Apr</t>
+  </si>
+  <si>
+    <t>3,791</t>
+  </si>
+  <si>
+    <t>USB,</t>
+  </si>
+  <si>
+    <t>2025-09-01T02:55:22.060628</t>
   </si>
 </sst>
 </file>
@@ -432,7 +675,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -468,31 +711,1297 @@
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
+      <c r="E8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
         <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" t="s">
+        <v>57</v>
+      </c>
+      <c r="H11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" t="s">
+        <v>60</v>
+      </c>
+      <c r="H14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" t="s">
+        <v>61</v>
+      </c>
+      <c r="H15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" t="s">
+        <v>62</v>
+      </c>
+      <c r="H16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" t="s">
+        <v>63</v>
+      </c>
+      <c r="H17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" t="s">
+        <v>64</v>
+      </c>
+      <c r="H18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" t="s">
+        <v>65</v>
+      </c>
+      <c r="H19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20" t="s">
+        <v>44</v>
+      </c>
+      <c r="G20" t="s">
+        <v>66</v>
+      </c>
+      <c r="H20" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" t="s">
+        <v>46</v>
+      </c>
+      <c r="G21" t="s">
+        <v>67</v>
+      </c>
+      <c r="H21" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F22" t="s">
+        <v>42</v>
+      </c>
+      <c r="G22" t="s">
+        <v>68</v>
+      </c>
+      <c r="H22" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23" t="s">
+        <v>42</v>
+      </c>
+      <c r="G23" t="s">
+        <v>69</v>
+      </c>
+      <c r="H23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" t="s">
+        <v>38</v>
+      </c>
+      <c r="F24" t="s">
+        <v>43</v>
+      </c>
+      <c r="G24" t="s">
+        <v>70</v>
+      </c>
+      <c r="H24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" t="s">
+        <v>38</v>
+      </c>
+      <c r="F25" t="s">
+        <v>45</v>
+      </c>
+      <c r="G25" t="s">
+        <v>71</v>
+      </c>
+      <c r="H25" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F26" t="s">
+        <v>39</v>
+      </c>
+      <c r="G26" t="s">
+        <v>72</v>
+      </c>
+      <c r="H26" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27" t="s">
+        <v>47</v>
+      </c>
+      <c r="G27" t="s">
+        <v>73</v>
+      </c>
+      <c r="H27" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" t="s">
+        <v>38</v>
+      </c>
+      <c r="F28" t="s">
+        <v>42</v>
+      </c>
+      <c r="G28" t="s">
+        <v>74</v>
+      </c>
+      <c r="H28" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" t="s">
+        <v>38</v>
+      </c>
+      <c r="F29" t="s">
+        <v>42</v>
+      </c>
+      <c r="G29" t="s">
+        <v>75</v>
+      </c>
+      <c r="H29" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" t="s">
+        <v>38</v>
+      </c>
+      <c r="F30" t="s">
+        <v>40</v>
+      </c>
+      <c r="G30" t="s">
+        <v>76</v>
+      </c>
+      <c r="H30" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" t="s">
+        <v>27</v>
+      </c>
+      <c r="E31" t="s">
+        <v>38</v>
+      </c>
+      <c r="F31" t="s">
+        <v>40</v>
+      </c>
+      <c r="G31" t="s">
+        <v>77</v>
+      </c>
+      <c r="H31" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" t="s">
+        <v>38</v>
+      </c>
+      <c r="F32" t="s">
+        <v>42</v>
+      </c>
+      <c r="G32" t="s">
+        <v>78</v>
+      </c>
+      <c r="H32" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F33" t="s">
+        <v>42</v>
+      </c>
+      <c r="G33" t="s">
+        <v>79</v>
+      </c>
+      <c r="H33" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" t="s">
+        <v>38</v>
+      </c>
+      <c r="F34" t="s">
+        <v>40</v>
+      </c>
+      <c r="G34" t="s">
+        <v>80</v>
+      </c>
+      <c r="H34" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" t="s">
+        <v>38</v>
+      </c>
+      <c r="F35" t="s">
+        <v>40</v>
+      </c>
+      <c r="G35" t="s">
+        <v>81</v>
+      </c>
+      <c r="H35" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" t="s">
+        <v>29</v>
+      </c>
+      <c r="E36" t="s">
+        <v>38</v>
+      </c>
+      <c r="F36" t="s">
+        <v>39</v>
+      </c>
+      <c r="G36" t="s">
+        <v>82</v>
+      </c>
+      <c r="H36" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" t="s">
+        <v>38</v>
+      </c>
+      <c r="F37" t="s">
+        <v>42</v>
+      </c>
+      <c r="G37" t="s">
+        <v>83</v>
+      </c>
+      <c r="H37" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" t="s">
+        <v>30</v>
+      </c>
+      <c r="E38" t="s">
+        <v>38</v>
+      </c>
+      <c r="F38" t="s">
+        <v>44</v>
+      </c>
+      <c r="G38" t="s">
+        <v>84</v>
+      </c>
+      <c r="H38" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" t="s">
+        <v>31</v>
+      </c>
+      <c r="E39" t="s">
+        <v>38</v>
+      </c>
+      <c r="F39" t="s">
+        <v>48</v>
+      </c>
+      <c r="G39" t="s">
+        <v>85</v>
+      </c>
+      <c r="H39" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" t="s">
+        <v>38</v>
+      </c>
+      <c r="F40" t="s">
+        <v>40</v>
+      </c>
+      <c r="G40" t="s">
+        <v>86</v>
+      </c>
+      <c r="H40" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" t="s">
+        <v>38</v>
+      </c>
+      <c r="F41" t="s">
+        <v>39</v>
+      </c>
+      <c r="G41" t="s">
+        <v>87</v>
+      </c>
+      <c r="H41" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" t="s">
+        <v>32</v>
+      </c>
+      <c r="E42" t="s">
+        <v>38</v>
+      </c>
+      <c r="F42" t="s">
+        <v>44</v>
+      </c>
+      <c r="G42" t="s">
+        <v>88</v>
+      </c>
+      <c r="H42" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" t="s">
+        <v>38</v>
+      </c>
+      <c r="F43" t="s">
+        <v>40</v>
+      </c>
+      <c r="G43" t="s">
+        <v>89</v>
+      </c>
+      <c r="H43" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" t="s">
+        <v>33</v>
+      </c>
+      <c r="E44" t="s">
+        <v>38</v>
+      </c>
+      <c r="F44" t="s">
+        <v>42</v>
+      </c>
+      <c r="G44" t="s">
+        <v>90</v>
+      </c>
+      <c r="H44" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E45" t="s">
+        <v>38</v>
+      </c>
+      <c r="F45" t="s">
+        <v>39</v>
+      </c>
+      <c r="G45" t="s">
+        <v>91</v>
+      </c>
+      <c r="H45" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" t="s">
+        <v>38</v>
+      </c>
+      <c r="F46" t="s">
+        <v>40</v>
+      </c>
+      <c r="G46" t="s">
+        <v>92</v>
+      </c>
+      <c r="H46" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" t="s">
+        <v>8</v>
+      </c>
+      <c r="B47" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D47" t="s">
+        <v>35</v>
+      </c>
+      <c r="E47" t="s">
+        <v>38</v>
+      </c>
+      <c r="F47" t="s">
+        <v>44</v>
+      </c>
+      <c r="G47" t="s">
+        <v>93</v>
+      </c>
+      <c r="H47" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D48" t="s">
+        <v>36</v>
+      </c>
+      <c r="E48" t="s">
+        <v>38</v>
+      </c>
+      <c r="F48" t="s">
+        <v>46</v>
+      </c>
+      <c r="G48" t="s">
+        <v>94</v>
+      </c>
+      <c r="H48" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D49" t="s">
+        <v>37</v>
+      </c>
+      <c r="E49" t="s">
+        <v>38</v>
+      </c>
+      <c r="F49" t="s">
+        <v>46</v>
+      </c>
+      <c r="G49" t="s">
+        <v>95</v>
+      </c>
+      <c r="H49" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
+    <hyperlink ref="C7" r:id="rId6"/>
+    <hyperlink ref="C8" r:id="rId7"/>
+    <hyperlink ref="C9" r:id="rId8"/>
+    <hyperlink ref="C10" r:id="rId9"/>
+    <hyperlink ref="C11" r:id="rId10"/>
+    <hyperlink ref="C12" r:id="rId11"/>
+    <hyperlink ref="C13" r:id="rId12"/>
+    <hyperlink ref="C14" r:id="rId13"/>
+    <hyperlink ref="C15" r:id="rId14"/>
+    <hyperlink ref="C16" r:id="rId15"/>
+    <hyperlink ref="C17" r:id="rId16"/>
+    <hyperlink ref="C18" r:id="rId17"/>
+    <hyperlink ref="C19" r:id="rId18"/>
+    <hyperlink ref="C20" r:id="rId19"/>
+    <hyperlink ref="C21" r:id="rId20"/>
+    <hyperlink ref="C22" r:id="rId21"/>
+    <hyperlink ref="C23" r:id="rId22"/>
+    <hyperlink ref="C24" r:id="rId23"/>
+    <hyperlink ref="C25" r:id="rId24"/>
+    <hyperlink ref="C26" r:id="rId25"/>
+    <hyperlink ref="C27" r:id="rId26"/>
+    <hyperlink ref="C28" r:id="rId27"/>
+    <hyperlink ref="C29" r:id="rId28"/>
+    <hyperlink ref="C30" r:id="rId29"/>
+    <hyperlink ref="C31" r:id="rId30"/>
+    <hyperlink ref="C32" r:id="rId31"/>
+    <hyperlink ref="C33" r:id="rId32"/>
+    <hyperlink ref="C34" r:id="rId33"/>
+    <hyperlink ref="C35" r:id="rId34"/>
+    <hyperlink ref="C36" r:id="rId35"/>
+    <hyperlink ref="C37" r:id="rId36"/>
+    <hyperlink ref="C38" r:id="rId37"/>
+    <hyperlink ref="C39" r:id="rId38"/>
+    <hyperlink ref="C40" r:id="rId39"/>
+    <hyperlink ref="C41" r:id="rId40"/>
+    <hyperlink ref="C42" r:id="rId41"/>
+    <hyperlink ref="C43" r:id="rId42"/>
+    <hyperlink ref="C44" r:id="rId43"/>
+    <hyperlink ref="C45" r:id="rId44"/>
+    <hyperlink ref="C46" r:id="rId45"/>
+    <hyperlink ref="C47" r:id="rId46"/>
+    <hyperlink ref="C48" r:id="rId47"/>
+    <hyperlink ref="C49" r:id="rId48"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>